<commit_message>
Added Data to US Crime Rates by State
</commit_message>
<xml_diff>
--- a/data/Crime_In_US_By_State/Crime_In_US_By_State_2018.xlsx
+++ b/data/Crime_In_US_By_State/Crime_In_US_By_State_2018.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D02F79F2-36F8-8E40-AE49-50CBC1F99F17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026594CF-95CD-BC40-A344-1EE62F3CCD89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1304,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
-      <selection activeCell="K1" sqref="A1:K1"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1317,7 +1317,7 @@
     <col min="5" max="5" width="19.1640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" style="2" customWidth="1"/>
     <col min="10" max="10" width="13.1640625" style="2" customWidth="1"/>
     <col min="11" max="11" width="11" style="2" customWidth="1"/>

</xml_diff>